<commit_message>
created my first attempt at loading a texture onto an image. You can see it in webGL-lessons/Lesson05
</commit_message>
<xml_diff>
--- a/status update James .xlsx
+++ b/status update James .xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="503" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="530" firstSheet="0" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Status Update 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,13 +29,14 @@
     <sheet name="Status Update 19" sheetId="19" state="visible" r:id="rId20"/>
     <sheet name="Status Update 20" sheetId="20" state="visible" r:id="rId21"/>
     <sheet name="Status Update 21" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Status Update 22" sheetId="22" state="visible" r:id="rId23"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="148">
   <si>
     <t>Current Status</t>
   </si>
@@ -474,6 +475,47 @@
   </si>
   <si>
     <t>Job 3:4 – Let that [the senior project] be darkness; let not God regard it from above, neither let the light shine upon it.</t>
+  </si>
+  <si>
+    <t>Worked on learning how to organize the project to make coding easier. Looked at shadows a bit more, and controls.</t>
+  </si>
+  <si>
+    <t>Still haven't found a house to move into after the semester is over.</t>
+  </si>
+  <si>
+    <t>On schedule</t>
+  </si>
+  <si>
+    <t>Will change my schedule to reflect this this week.</t>
+  </si>
+  <si>
+    <t>Need to finish changing my schedule to reflect my actual timeline.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Abraham 4:14 - And [James] </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12.1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">organized</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> the lights in the expanse of the [virtual] heaven, and caused them to divide the day from the night;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6780,8 +6822,8 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7193,6 +7235,468 @@
       <c r="B17" s="47"/>
       <c r="C17" s="48" t="s">
         <v>141</v>
+      </c>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:K13"/>
+    <mergeCell ref="A14:B16"/>
+    <mergeCell ref="C14:K14"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="C16:K16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:K17"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2955465587045"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2874493927126"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.2914979757085"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.71255060728745"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.2914979757085"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.7246963562753"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="41"/>
+      <c r="B1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="44"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="28" t="n">
+        <v>41699</v>
+      </c>
+      <c r="D3" s="28" t="n">
+        <v>41699</v>
+      </c>
+      <c r="E3" s="28" t="n">
+        <v>41699</v>
+      </c>
+      <c r="F3" s="28" t="n">
+        <v>41765</v>
+      </c>
+      <c r="G3" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="H3" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="I3" s="29" t="n">
+        <v>5</v>
+      </c>
+      <c r="J3" s="29" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" s="29" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="D4" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="E4" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="F4" s="28" t="n">
+        <v>41768</v>
+      </c>
+      <c r="G4" s="28" t="n">
+        <v>41768</v>
+      </c>
+      <c r="H4" s="28" t="n">
+        <v>41772</v>
+      </c>
+      <c r="I4" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" s="29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="D5" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="E5" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="F5" s="28" t="n">
+        <v>41768</v>
+      </c>
+      <c r="G5" s="28" t="n">
+        <v>41768</v>
+      </c>
+      <c r="H5" s="28" t="n">
+        <v>41772</v>
+      </c>
+      <c r="I5" s="29" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" s="29" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" s="29" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="28" t="n">
+        <v>41773</v>
+      </c>
+      <c r="D6" s="28" t="n">
+        <v>41713</v>
+      </c>
+      <c r="E6" s="28" t="n">
+        <v>41713</v>
+      </c>
+      <c r="F6" s="28" t="n">
+        <v>41809</v>
+      </c>
+      <c r="G6" s="28" t="n">
+        <v>41823</v>
+      </c>
+      <c r="H6" s="28" t="n">
+        <v>41830</v>
+      </c>
+      <c r="I6" s="29" t="n">
+        <v>60</v>
+      </c>
+      <c r="J6" s="29" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="K6" s="29" t="n">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="28" t="n">
+        <v>41810</v>
+      </c>
+      <c r="D7" s="28" t="n">
+        <v>41830</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="28" t="n">
+        <v>41845</v>
+      </c>
+      <c r="G7" s="28" t="n">
+        <v>41907</v>
+      </c>
+      <c r="H7" s="31"/>
+      <c r="I7" s="29" t="n">
+        <v>50</v>
+      </c>
+      <c r="J7" s="29" t="n">
+        <v>63</v>
+      </c>
+      <c r="K7" s="29" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="28" t="n">
+        <v>42024</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="28" t="n">
+        <v>42060</v>
+      </c>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="28" t="n">
+        <v>42068</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="28" t="n">
+        <v>42088</v>
+      </c>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="29" t="n">
+        <v>189</v>
+      </c>
+      <c r="J10" s="29" t="n">
+        <v>181.5</v>
+      </c>
+      <c r="K10" s="29" t="n">
+        <f aca="false">SUM(K3:K9)</f>
+        <v>130.5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+    </row>
+    <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+    </row>
+    <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="42"/>
+      <c r="C13" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="47"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+    </row>
+    <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+    </row>
+    <row r="17" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48" t="s">
+        <v>147</v>
       </c>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>

</xml_diff>

<commit_message>
modified lesson07 with comments to be able to reference later when actual coding begins
</commit_message>
<xml_diff>
--- a/status update James .xlsx
+++ b/status update James .xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="24"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Status Update 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,13 +33,14 @@
     <sheet name="Status Update 23" sheetId="23" state="visible" r:id="rId24"/>
     <sheet name="Status Update 24" sheetId="24" state="visible" r:id="rId25"/>
     <sheet name="Status Update 25" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="Status Update 26" sheetId="26" state="visible" r:id="rId27"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="166">
   <si>
     <t>Current Status</t>
   </si>
@@ -558,6 +559,21 @@
   </si>
   <si>
     <t>Mosiah 18:32 - But behold, it came to pass that the [student], having discovered a movement among [his project], [was excited because he had been working on it for a while].</t>
+  </si>
+  <si>
+    <t>Achieved movement, the ability to change the ambient lighting color, and the ability to change the direction the lighting is coming from.</t>
+  </si>
+  <si>
+    <t>Still have quite a bit of design to go</t>
+  </si>
+  <si>
+    <t>Going to have most of my research/design if not all finished 2 weeks from now, and start on coding the actual project.</t>
+  </si>
+  <si>
+    <t>Things are progressing well so far.</t>
+  </si>
+  <si>
+    <t>Alma 43:7 - ...that he might bring [webgl] into subjection to the accomplishment of his designs.</t>
   </si>
 </sst>
 </file>
@@ -8710,8 +8726,8 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -9125,6 +9141,468 @@
       <c r="B17" s="47"/>
       <c r="C17" s="48" t="s">
         <v>160</v>
+      </c>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:K13"/>
+    <mergeCell ref="A14:B16"/>
+    <mergeCell ref="C14:K14"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="C16:K16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:K17"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2908163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="10.719387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.71428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.71938775510204"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="41"/>
+      <c r="B1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="44"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="28" t="n">
+        <v>41699</v>
+      </c>
+      <c r="D3" s="28" t="n">
+        <v>41699</v>
+      </c>
+      <c r="E3" s="28" t="n">
+        <v>41699</v>
+      </c>
+      <c r="F3" s="28" t="n">
+        <v>41765</v>
+      </c>
+      <c r="G3" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="H3" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="I3" s="29" t="n">
+        <v>5</v>
+      </c>
+      <c r="J3" s="29" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" s="29" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="D4" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="E4" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="F4" s="28" t="n">
+        <v>41768</v>
+      </c>
+      <c r="G4" s="28" t="n">
+        <v>41768</v>
+      </c>
+      <c r="H4" s="28" t="n">
+        <v>41772</v>
+      </c>
+      <c r="I4" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" s="29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="D5" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="E5" s="28" t="n">
+        <v>41766</v>
+      </c>
+      <c r="F5" s="28" t="n">
+        <v>41768</v>
+      </c>
+      <c r="G5" s="28" t="n">
+        <v>41768</v>
+      </c>
+      <c r="H5" s="28" t="n">
+        <v>41772</v>
+      </c>
+      <c r="I5" s="29" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" s="29" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" s="29" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="28" t="n">
+        <v>41773</v>
+      </c>
+      <c r="D6" s="28" t="n">
+        <v>41713</v>
+      </c>
+      <c r="E6" s="28" t="n">
+        <v>41713</v>
+      </c>
+      <c r="F6" s="28" t="n">
+        <v>41809</v>
+      </c>
+      <c r="G6" s="28" t="n">
+        <v>41823</v>
+      </c>
+      <c r="H6" s="28" t="n">
+        <v>41830</v>
+      </c>
+      <c r="I6" s="29" t="n">
+        <v>60</v>
+      </c>
+      <c r="J6" s="29" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="K6" s="29" t="n">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="28" t="n">
+        <v>41810</v>
+      </c>
+      <c r="D7" s="28" t="n">
+        <v>41830</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="28" t="n">
+        <v>41845</v>
+      </c>
+      <c r="G7" s="28" t="n">
+        <v>41907</v>
+      </c>
+      <c r="H7" s="31"/>
+      <c r="I7" s="29" t="n">
+        <v>50</v>
+      </c>
+      <c r="J7" s="29" t="n">
+        <v>76</v>
+      </c>
+      <c r="K7" s="29" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="28" t="n">
+        <v>42024</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="28" t="n">
+        <v>42060</v>
+      </c>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="28" t="n">
+        <v>42068</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="28" t="n">
+        <v>42088</v>
+      </c>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="29" t="n">
+        <v>189</v>
+      </c>
+      <c r="J10" s="29" t="n">
+        <v>208</v>
+      </c>
+      <c r="K10" s="29" t="n">
+        <f aca="false">SUM(K3:K9)</f>
+        <v>143.5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+    </row>
+    <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+    </row>
+    <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="42"/>
+      <c r="C13" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="51" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="47"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+    </row>
+    <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+    </row>
+    <row r="17" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48" t="s">
+        <v>165</v>
       </c>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>

</xml_diff>